<commit_message>
bugfix de memoria e typecast de floats no win32
</commit_message>
<xml_diff>
--- a/aa-trabalho1-20111/timings.xlsx
+++ b/aa-trabalho1-20111/timings.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr date1904="1" showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16600" tabRatio="500"/>
   </bookViews>
@@ -653,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A51" zoomScale="150" workbookViewId="0">
       <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
@@ -2122,6 +2122,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.51388888888888884" right="0.40277777777777779" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>